<commit_message>
Base de datos reparada
</commit_message>
<xml_diff>
--- a/DataBase/Consumos/consumos_COSTAVERDE_18_01_2026.xlsx
+++ b/DataBase/Consumos/consumos_COSTAVERDE_18_01_2026.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
-  <x:si>
-    <x:t>Desde: 01/01/2026 Hasta: 17/01/2026</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
+  <x:si>
+    <x:t>Desde: 01/01/2026 Hasta: 18/01/2026</x:t>
   </x:si>
   <x:si>
     <x:t>Sucursales: COSTAVERDE</x:t>
@@ -284,6 +284,15 @@
   </x:si>
   <x:si>
     <x:t>PASTELERIA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COOKIE MANTECOL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COOKIE OREO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BUDIN LIMON</x:t>
   </x:si>
   <x:si>
     <x:t>ALFAJOR DE ALMENDRAS</x:t>
@@ -683,8 +692,8 @@
 </file>
 
 <file path=xl/tables/table.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E182" totalsRowShown="0">
-  <x:autoFilter ref="A4:E182"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E185" totalsRowShown="0">
+  <x:autoFilter ref="A4:E185"/>
   <x:tableColumns count="5">
     <x:tableColumn id="1" name="FAMILIA"/>
     <x:tableColumn id="2" name="CODIGO"/>
@@ -984,7 +993,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E182"/>
+  <x:dimension ref="A1:E185"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1039,10 +1048,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
-        <x:v>226</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>971800</x:v>
+        <x:v>984700</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
@@ -1056,10 +1065,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
-        <x:v>102</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>581400</x:v>
+        <x:v>609900</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
@@ -1073,10 +1082,10 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D7" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>145400</x:v>
+        <x:v>150800</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
@@ -1090,10 +1099,10 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="D8" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E8" s="0" t="n">
-        <x:v>79200</x:v>
+        <x:v>92000</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
@@ -1107,10 +1116,10 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="D9" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E9" s="0" t="n">
-        <x:v>89100</x:v>
+        <x:v>99600</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
@@ -1124,10 +1133,10 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="D10" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
-        <x:v>74850</x:v>
+        <x:v>86850</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
@@ -1192,10 +1201,10 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="D14" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
-        <x:v>261000</x:v>
+        <x:v>366000</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
@@ -1277,10 +1286,10 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="D19" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="E19" s="0" t="n">
-        <x:v>427300</x:v>
+        <x:v>441100</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
@@ -1294,10 +1303,10 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="D20" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
-        <x:v>818900</x:v>
+        <x:v>848400</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5">
@@ -1328,10 +1337,10 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="D22" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
-        <x:v>87100</x:v>
+        <x:v>100500</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
@@ -1413,10 +1422,10 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="D27" s="0" t="n">
-        <x:v>101</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
-        <x:v>333300</x:v>
+        <x:v>346500</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:5">
@@ -1430,10 +1439,10 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="D28" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
-        <x:v>456300</x:v>
+        <x:v>464100</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:5">
@@ -1464,10 +1473,10 @@
         <x:v>37</x:v>
       </x:c>
       <x:c r="D30" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
-        <x:v>377300</x:v>
+        <x:v>382200</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:5">
@@ -1532,10 +1541,10 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="D34" s="0" t="n">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
-        <x:v>638500</x:v>
+        <x:v>654900</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:5">
@@ -1566,10 +1575,10 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="D36" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
-        <x:v>531300</x:v>
+        <x:v>540900</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:5">
@@ -1583,10 +1592,10 @@
         <x:v>45</x:v>
       </x:c>
       <x:c r="D37" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
-        <x:v>513500</x:v>
+        <x:v>539500</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:5">
@@ -1617,10 +1626,10 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="D39" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
-        <x:v>257300</x:v>
+        <x:v>265600</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:5">
@@ -1651,10 +1660,10 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="D41" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>139600</x:v>
+        <x:v>157200</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:5">
@@ -1753,10 +1762,10 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="D47" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
-        <x:v>507100</x:v>
+        <x:v>546100</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:5">
@@ -1770,10 +1779,10 @@
         <x:v>59</x:v>
       </x:c>
       <x:c r="D48" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>220500</x:v>
+        <x:v>270900</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:5">
@@ -1787,10 +1796,10 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="D49" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>82900</x:v>
+        <x:v>106600</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:5">
@@ -1821,10 +1830,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="D51" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
-        <x:v>100600</x:v>
+        <x:v>124300</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:5">
@@ -1838,10 +1847,10 @@
         <x:v>63</x:v>
       </x:c>
       <x:c r="D52" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
-        <x:v>120400</x:v>
+        <x:v>144100</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:5">
@@ -1906,10 +1915,10 @@
         <x:v>69</x:v>
       </x:c>
       <x:c r="D56" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E56" s="0" t="n">
-        <x:v>55200</x:v>
+        <x:v>62100</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:5">
@@ -1940,10 +1949,10 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="D58" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E58" s="0" t="n">
-        <x:v>93500</x:v>
+        <x:v>110500</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:5">
@@ -1991,10 +2000,10 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="D61" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E61" s="0" t="n">
-        <x:v>43500</x:v>
+        <x:v>52200</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:5">
@@ -2025,10 +2034,10 @@
         <x:v>76</x:v>
       </x:c>
       <x:c r="D63" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E63" s="0" t="n">
-        <x:v>19000</x:v>
+        <x:v>38000</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:5">
@@ -2059,10 +2068,10 @@
         <x:v>78</x:v>
       </x:c>
       <x:c r="D65" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E65" s="0" t="n">
-        <x:v>212700</x:v>
+        <x:v>226500</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:5">
@@ -2076,10 +2085,10 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="D66" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E66" s="0" t="n">
-        <x:v>145200</x:v>
+        <x:v>149600</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:5">
@@ -2127,10 +2136,10 @@
         <x:v>84</x:v>
       </x:c>
       <x:c r="D69" s="0" t="n">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="E69" s="0" t="n">
-        <x:v>927600</x:v>
+        <x:v>936300</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:5">
@@ -2144,10 +2153,10 @@
         <x:v>85</x:v>
       </x:c>
       <x:c r="D70" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E70" s="0" t="n">
-        <x:v>106600</x:v>
+        <x:v>113800</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:5">
@@ -2161,10 +2170,10 @@
         <x:v>86</x:v>
       </x:c>
       <x:c r="D71" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="E71" s="0" t="n">
-        <x:v>209600</x:v>
+        <x:v>217200</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:5">
@@ -2178,10 +2187,10 @@
         <x:v>87</x:v>
       </x:c>
       <x:c r="D72" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E72" s="0" t="n">
-        <x:v>60000</x:v>
+        <x:v>67600</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:5">
@@ -2206,16 +2215,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B74" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C74" s="0" t="s">
         <x:v>90</x:v>
       </x:c>
       <x:c r="D74" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E74" s="0" t="n">
-        <x:v>11000</x:v>
+        <x:v>5100</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:5">
@@ -2223,16 +2232,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B75" s="0" t="n">
-        <x:v>42</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C75" s="0" t="s">
         <x:v>91</x:v>
       </x:c>
       <x:c r="D75" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E75" s="0" t="n">
-        <x:v>28200</x:v>
+        <x:v>5100</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:5">
@@ -2240,16 +2249,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B76" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C76" s="0" t="s">
         <x:v>92</x:v>
       </x:c>
       <x:c r="D76" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E76" s="0" t="n">
-        <x:v>68400</x:v>
+        <x:v>5500</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:5">
@@ -2257,16 +2266,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B77" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C77" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="D77" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E77" s="0" t="n">
-        <x:v>39920</x:v>
+        <x:v>11000</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:5">
@@ -2274,16 +2283,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B78" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C78" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D78" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
       <x:c r="E78" s="0" t="n">
-        <x:v>30600</x:v>
+        <x:v>28200</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:5">
@@ -2291,16 +2300,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B79" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C79" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="D79" s="0" t="n">
-        <x:v>319</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E79" s="0" t="n">
-        <x:v>542300</x:v>
+        <x:v>68400</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:5">
@@ -2308,10 +2317,10 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B80" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C80" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="D80" s="0" t="n">
         <x:v>8</x:v>
@@ -2325,16 +2334,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B81" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C81" s="0" t="s">
         <x:v>96</x:v>
       </x:c>
       <x:c r="D81" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E81" s="0" t="n">
-        <x:v>90200</x:v>
+        <x:v>30600</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:5">
@@ -2342,16 +2351,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B82" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C82" s="0" t="s">
         <x:v>97</x:v>
       </x:c>
       <x:c r="D82" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="E82" s="0" t="n">
-        <x:v>84830</x:v>
+        <x:v>547400</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:5">
@@ -2359,16 +2368,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B83" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C83" s="0" t="s">
         <x:v>98</x:v>
       </x:c>
       <x:c r="D83" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E83" s="0" t="n">
-        <x:v>79500</x:v>
+        <x:v>39920</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:5">
@@ -2376,16 +2385,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B84" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C84" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="D84" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E84" s="0" t="n">
-        <x:v>79900</x:v>
+        <x:v>90200</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:5">
@@ -2393,16 +2402,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B85" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C85" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="D85" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E85" s="0" t="n">
-        <x:v>172500</x:v>
+        <x:v>84830</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:5">
@@ -2410,16 +2419,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B86" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C86" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="D86" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E86" s="0" t="n">
-        <x:v>66000</x:v>
+        <x:v>84800</x:v>
       </x:c>
     </x:row>
     <x:row r="87" spans="1:5">
@@ -2427,16 +2436,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B87" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C87" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D87" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E87" s="0" t="n">
-        <x:v>59880</x:v>
+        <x:v>79900</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:5">
@@ -2444,16 +2453,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B88" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C88" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="D88" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E88" s="0" t="n">
-        <x:v>104500</x:v>
+        <x:v>172500</x:v>
       </x:c>
     </x:row>
     <x:row r="89" spans="1:5">
@@ -2461,16 +2470,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B89" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C89" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="D89" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E89" s="0" t="n">
-        <x:v>33600</x:v>
+        <x:v>66000</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:5">
@@ -2478,16 +2487,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B90" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C90" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="D90" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E90" s="0" t="n">
-        <x:v>49500</x:v>
+        <x:v>59880</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:5">
@@ -2495,16 +2504,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B91" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C91" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="D91" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E91" s="0" t="n">
-        <x:v>125400</x:v>
+        <x:v>115500</x:v>
       </x:c>
     </x:row>
     <x:row r="92" spans="1:5">
@@ -2512,16 +2521,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B92" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C92" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="D92" s="0" t="n">
         <x:v>7</x:v>
       </x:c>
       <x:c r="E92" s="0" t="n">
-        <x:v>31500</x:v>
+        <x:v>33600</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:5">
@@ -2529,16 +2538,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B93" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C93" s="0" t="s">
         <x:v>105</x:v>
       </x:c>
       <x:c r="D93" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E93" s="0" t="n">
-        <x:v>35500</x:v>
+        <x:v>58500</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:5">
@@ -2546,16 +2555,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B94" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C94" s="0" t="s">
         <x:v>106</x:v>
       </x:c>
       <x:c r="D94" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E94" s="0" t="n">
-        <x:v>65600</x:v>
+        <x:v>125400</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:5">
@@ -2563,16 +2572,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B95" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C95" s="0" t="s">
         <x:v>107</x:v>
       </x:c>
       <x:c r="D95" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E95" s="0" t="n">
-        <x:v>112500</x:v>
+        <x:v>36000</x:v>
       </x:c>
     </x:row>
     <x:row r="96" spans="1:5">
@@ -2580,16 +2589,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B96" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C96" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="D96" s="0" t="n">
         <x:v>5</x:v>
       </x:c>
       <x:c r="E96" s="0" t="n">
-        <x:v>27500</x:v>
+        <x:v>35500</x:v>
       </x:c>
     </x:row>
     <x:row r="97" spans="1:5">
@@ -2597,16 +2606,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B97" s="0" t="n">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C97" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="D97" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E97" s="0" t="n">
-        <x:v>52500</x:v>
+        <x:v>65600</x:v>
       </x:c>
     </x:row>
     <x:row r="98" spans="1:5">
@@ -2614,16 +2623,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B98" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C98" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="D98" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E98" s="0" t="n">
-        <x:v>49600</x:v>
+        <x:v>112500</x:v>
       </x:c>
     </x:row>
     <x:row r="99" spans="1:5">
@@ -2631,16 +2640,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B99" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C99" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="D99" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E99" s="0" t="n">
-        <x:v>28800</x:v>
+        <x:v>27500</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:5">
@@ -2648,16 +2657,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B100" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C100" s="0" t="s">
         <x:v>111</x:v>
       </x:c>
       <x:c r="D100" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E100" s="0" t="n">
-        <x:v>80400</x:v>
+        <x:v>60000</x:v>
       </x:c>
     </x:row>
     <x:row r="101" spans="1:5">
@@ -2665,16 +2674,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B101" s="0" t="n">
-        <x:v>63</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C101" s="0" t="s">
         <x:v>112</x:v>
       </x:c>
       <x:c r="D101" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E101" s="0" t="n">
-        <x:v>66500</x:v>
+        <x:v>49600</x:v>
       </x:c>
     </x:row>
     <x:row r="102" spans="1:5">
@@ -2682,16 +2691,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B102" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C102" s="0" t="s">
         <x:v>113</x:v>
       </x:c>
       <x:c r="D102" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E102" s="0" t="n">
-        <x:v>15900</x:v>
+        <x:v>43700</x:v>
       </x:c>
     </x:row>
     <x:row r="103" spans="1:5">
@@ -2699,16 +2708,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B103" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C103" s="0" t="s">
         <x:v>114</x:v>
       </x:c>
       <x:c r="D103" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E103" s="0" t="n">
-        <x:v>13900</x:v>
+        <x:v>80400</x:v>
       </x:c>
     </x:row>
     <x:row r="104" spans="1:5">
@@ -2716,7 +2725,7 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B104" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C104" s="0" t="s">
         <x:v>115</x:v>
@@ -2725,7 +2734,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E104" s="0" t="n">
-        <x:v>70500</x:v>
+        <x:v>66500</x:v>
       </x:c>
     </x:row>
     <x:row r="105" spans="1:5">
@@ -2733,7 +2742,7 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B105" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C105" s="0" t="s">
         <x:v>116</x:v>
@@ -2742,7 +2751,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="E105" s="0" t="n">
-        <x:v>30800</x:v>
+        <x:v>31800</x:v>
       </x:c>
     </x:row>
     <x:row r="106" spans="1:5">
@@ -2750,16 +2759,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B106" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C106" s="0" t="s">
         <x:v>117</x:v>
       </x:c>
       <x:c r="D106" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E106" s="0" t="n">
-        <x:v>32400</x:v>
+        <x:v>13900</x:v>
       </x:c>
     </x:row>
     <x:row r="107" spans="1:5">
@@ -2767,16 +2776,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B107" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C107" s="0" t="s">
         <x:v>118</x:v>
       </x:c>
       <x:c r="D107" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E107" s="0" t="n">
-        <x:v>6400</x:v>
+        <x:v>85400</x:v>
       </x:c>
     </x:row>
     <x:row r="108" spans="1:5">
@@ -2784,16 +2793,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B108" s="0" t="n">
-        <x:v>601</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C108" s="0" t="s">
         <x:v>119</x:v>
       </x:c>
       <x:c r="D108" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E108" s="0" t="n">
-        <x:v>35800</x:v>
+        <x:v>30800</x:v>
       </x:c>
     </x:row>
     <x:row r="109" spans="1:5">
@@ -2801,16 +2810,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B109" s="0" t="n">
-        <x:v>602</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C109" s="0" t="s">
         <x:v>120</x:v>
       </x:c>
       <x:c r="D109" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E109" s="0" t="n">
-        <x:v>136200</x:v>
+        <x:v>32400</x:v>
       </x:c>
     </x:row>
     <x:row r="110" spans="1:5">
@@ -2818,16 +2827,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B110" s="0" t="n">
-        <x:v>603</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C110" s="0" t="s">
         <x:v>121</x:v>
       </x:c>
       <x:c r="D110" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E110" s="0" t="n">
-        <x:v>90900</x:v>
+        <x:v>6400</x:v>
       </x:c>
     </x:row>
     <x:row r="111" spans="1:5">
@@ -2835,16 +2844,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B111" s="0" t="n">
-        <x:v>604</x:v>
+        <x:v>601</x:v>
       </x:c>
       <x:c r="C111" s="0" t="s">
         <x:v>122</x:v>
       </x:c>
       <x:c r="D111" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E111" s="0" t="n">
-        <x:v>62700</x:v>
+        <x:v>35800</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="1:5">
@@ -2852,16 +2861,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B112" s="0" t="n">
-        <x:v>605</x:v>
+        <x:v>602</x:v>
       </x:c>
       <x:c r="C112" s="0" t="s">
         <x:v>123</x:v>
       </x:c>
       <x:c r="D112" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E112" s="0" t="n">
-        <x:v>120600</x:v>
+        <x:v>171000</x:v>
       </x:c>
     </x:row>
     <x:row r="113" spans="1:5">
@@ -2869,16 +2878,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B113" s="0" t="n">
-        <x:v>606</x:v>
+        <x:v>603</x:v>
       </x:c>
       <x:c r="C113" s="0" t="s">
         <x:v>124</x:v>
       </x:c>
       <x:c r="D113" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E113" s="0" t="n">
-        <x:v>125000</x:v>
+        <x:v>90900</x:v>
       </x:c>
     </x:row>
     <x:row r="114" spans="1:5">
@@ -2886,16 +2895,16 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B114" s="0" t="n">
-        <x:v>607</x:v>
+        <x:v>604</x:v>
       </x:c>
       <x:c r="C114" s="0" t="s">
         <x:v>125</x:v>
       </x:c>
       <x:c r="D114" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E114" s="0" t="n">
-        <x:v>38000</x:v>
+        <x:v>81300</x:v>
       </x:c>
     </x:row>
     <x:row r="115" spans="1:5">
@@ -2903,203 +2912,203 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="B115" s="0" t="n">
-        <x:v>608</x:v>
+        <x:v>605</x:v>
       </x:c>
       <x:c r="C115" s="0" t="s">
         <x:v>126</x:v>
       </x:c>
       <x:c r="D115" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E115" s="0" t="n">
-        <x:v>19800</x:v>
+        <x:v>138000</x:v>
       </x:c>
     </x:row>
     <x:row r="116" spans="1:5">
       <x:c r="A116" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B116" s="0" t="n">
+        <x:v>606</x:v>
+      </x:c>
+      <x:c r="C116" s="0" t="s">
         <x:v>127</x:v>
       </x:c>
-      <x:c r="B116" s="0" t="n">
-        <x:v>263</x:v>
-      </x:c>
-      <x:c r="C116" s="0" t="s">
-        <x:v>128</x:v>
-      </x:c>
       <x:c r="D116" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E116" s="0" t="n">
-        <x:v>67200</x:v>
+        <x:v>125000</x:v>
       </x:c>
     </x:row>
     <x:row r="117" spans="1:5">
       <x:c r="A117" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="B117" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>607</x:v>
       </x:c>
       <x:c r="C117" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="D117" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E117" s="0" t="n">
-        <x:v>14400</x:v>
+        <x:v>38000</x:v>
       </x:c>
     </x:row>
     <x:row r="118" spans="1:5">
       <x:c r="A118" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B118" s="0" t="n">
+        <x:v>608</x:v>
+      </x:c>
+      <x:c r="C118" s="0" t="s">
         <x:v>129</x:v>
       </x:c>
-      <x:c r="B118" s="0" t="n">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="C118" s="0" t="s">
-        <x:v>131</x:v>
-      </x:c>
       <x:c r="D118" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E118" s="0" t="n">
-        <x:v>32500</x:v>
+        <x:v>19800</x:v>
       </x:c>
     </x:row>
     <x:row r="119" spans="1:5">
       <x:c r="A119" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="B119" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="C119" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="D119" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E119" s="0" t="n">
-        <x:v>14000</x:v>
+        <x:v>75600</x:v>
       </x:c>
     </x:row>
     <x:row r="120" spans="1:5">
       <x:c r="A120" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B120" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C120" s="0" t="s">
         <x:v>133</x:v>
       </x:c>
       <x:c r="D120" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E120" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>14400</x:v>
       </x:c>
     </x:row>
     <x:row r="121" spans="1:5">
       <x:c r="A121" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B121" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C121" s="0" t="s">
         <x:v>134</x:v>
       </x:c>
       <x:c r="D121" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E121" s="0" t="n">
-        <x:v>76300</x:v>
+        <x:v>32500</x:v>
       </x:c>
     </x:row>
     <x:row r="122" spans="1:5">
       <x:c r="A122" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B122" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C122" s="0" t="s">
         <x:v>135</x:v>
       </x:c>
       <x:c r="D122" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E122" s="0" t="n">
-        <x:v>41300</x:v>
+        <x:v>14000</x:v>
       </x:c>
     </x:row>
     <x:row r="123" spans="1:5">
       <x:c r="A123" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B123" s="0" t="n">
-        <x:v>504</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="C123" s="0" t="s">
         <x:v>136</x:v>
       </x:c>
       <x:c r="D123" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E123" s="0" t="n">
-        <x:v>416500</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="124" spans="1:5">
       <x:c r="A124" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B124" s="0" t="n">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="C124" s="0" t="s">
         <x:v>137</x:v>
       </x:c>
-      <x:c r="B124" s="0" t="n">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="C124" s="0" t="s">
-        <x:v>138</x:v>
-      </x:c>
       <x:c r="D124" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E124" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>87200</x:v>
       </x:c>
     </x:row>
     <x:row r="125" spans="1:5">
       <x:c r="A125" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B125" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C125" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="D125" s="0" t="n">
-        <x:v>407</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E125" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>41300</x:v>
       </x:c>
     </x:row>
     <x:row r="126" spans="1:5">
       <x:c r="A126" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="B126" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>504</x:v>
       </x:c>
       <x:c r="C126" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="D126" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E126" s="0" t="n">
-        <x:v>45500</x:v>
+        <x:v>416500</x:v>
       </x:c>
     </x:row>
     <x:row r="127" spans="1:5">
@@ -3107,7 +3116,7 @@
         <x:v>140</x:v>
       </x:c>
       <x:c r="B127" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C127" s="0" t="s">
         <x:v>141</x:v>
@@ -3116,7 +3125,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="E127" s="0" t="n">
-        <x:v>3000</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="128" spans="1:5">
@@ -3124,211 +3133,211 @@
         <x:v>140</x:v>
       </x:c>
       <x:c r="B128" s="0" t="n">
-        <x:v>30</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C128" s="0" t="s">
         <x:v>142</x:v>
       </x:c>
       <x:c r="D128" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>446</x:v>
       </x:c>
       <x:c r="E128" s="0" t="n">
-        <x:v>177100</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="129" spans="1:5">
       <x:c r="A129" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B129" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C129" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="D129" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E129" s="0" t="n">
-        <x:v>370500</x:v>
+        <x:v>45500</x:v>
       </x:c>
     </x:row>
     <x:row r="130" spans="1:5">
       <x:c r="A130" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B130" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C130" s="0" t="s">
         <x:v>144</x:v>
       </x:c>
       <x:c r="D130" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E130" s="0" t="n">
-        <x:v>185300</x:v>
+        <x:v>3000</x:v>
       </x:c>
     </x:row>
     <x:row r="131" spans="1:5">
       <x:c r="A131" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B131" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C131" s="0" t="s">
         <x:v>145</x:v>
       </x:c>
       <x:c r="D131" s="0" t="n">
-        <x:v>54</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E131" s="0" t="n">
-        <x:v>588600</x:v>
+        <x:v>177100</x:v>
       </x:c>
     </x:row>
     <x:row r="132" spans="1:5">
       <x:c r="A132" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B132" s="0" t="n">
-        <x:v>35</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C132" s="0" t="s">
         <x:v>146</x:v>
       </x:c>
       <x:c r="D132" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E132" s="0" t="n">
-        <x:v>156600</x:v>
+        <x:v>370500</x:v>
       </x:c>
     </x:row>
     <x:row r="133" spans="1:5">
       <x:c r="A133" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B133" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C133" s="0" t="s">
         <x:v>147</x:v>
       </x:c>
       <x:c r="D133" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E133" s="0" t="n">
-        <x:v>119900</x:v>
+        <x:v>185300</x:v>
       </x:c>
     </x:row>
     <x:row r="134" spans="1:5">
       <x:c r="A134" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B134" s="0" t="n">
-        <x:v>37</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C134" s="0" t="s">
         <x:v>148</x:v>
       </x:c>
       <x:c r="D134" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E134" s="0" t="n">
-        <x:v>158400</x:v>
+        <x:v>588600</x:v>
       </x:c>
     </x:row>
     <x:row r="135" spans="1:5">
       <x:c r="A135" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B135" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C135" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="D135" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E135" s="0" t="n">
-        <x:v>59500</x:v>
+        <x:v>156600</x:v>
       </x:c>
     </x:row>
     <x:row r="136" spans="1:5">
       <x:c r="A136" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B136" s="0" t="n">
-        <x:v>400</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C136" s="0" t="s">
         <x:v>150</x:v>
       </x:c>
       <x:c r="D136" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E136" s="0" t="n">
-        <x:v>16100</x:v>
+        <x:v>119900</x:v>
       </x:c>
     </x:row>
     <x:row r="137" spans="1:5">
       <x:c r="A137" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B137" s="0" t="n">
-        <x:v>401</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C137" s="0" t="s">
         <x:v>151</x:v>
       </x:c>
       <x:c r="D137" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E137" s="0" t="n">
-        <x:v>3800</x:v>
+        <x:v>158400</x:v>
       </x:c>
     </x:row>
     <x:row r="138" spans="1:5">
       <x:c r="A138" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B138" s="0" t="n">
-        <x:v>403</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C138" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="D138" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E138" s="0" t="n">
-        <x:v>10000</x:v>
+        <x:v>59500</x:v>
       </x:c>
     </x:row>
     <x:row r="139" spans="1:5">
       <x:c r="A139" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B139" s="0" t="n">
-        <x:v>404</x:v>
+        <x:v>400</x:v>
       </x:c>
       <x:c r="C139" s="0" t="s">
         <x:v>153</x:v>
       </x:c>
       <x:c r="D139" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E139" s="0" t="n">
-        <x:v>8000</x:v>
+        <x:v>20700</x:v>
       </x:c>
     </x:row>
     <x:row r="140" spans="1:5">
       <x:c r="A140" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B140" s="0" t="n">
-        <x:v>405</x:v>
+        <x:v>401</x:v>
       </x:c>
       <x:c r="C140" s="0" t="s">
         <x:v>154</x:v>
@@ -3337,245 +3346,245 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="E140" s="0" t="n">
-        <x:v>1700</x:v>
+        <x:v>3800</x:v>
       </x:c>
     </x:row>
     <x:row r="141" spans="1:5">
       <x:c r="A141" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B141" s="0" t="n">
-        <x:v>411</x:v>
+        <x:v>403</x:v>
       </x:c>
       <x:c r="C141" s="0" t="s">
         <x:v>155</x:v>
       </x:c>
       <x:c r="D141" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E141" s="0" t="n">
-        <x:v>18000</x:v>
+        <x:v>10000</x:v>
       </x:c>
     </x:row>
     <x:row r="142" spans="1:5">
       <x:c r="A142" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B142" s="0" t="n">
-        <x:v>412</x:v>
+        <x:v>404</x:v>
       </x:c>
       <x:c r="C142" s="0" t="s">
         <x:v>156</x:v>
       </x:c>
       <x:c r="D142" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E142" s="0" t="n">
-        <x:v>25500</x:v>
+        <x:v>8000</x:v>
       </x:c>
     </x:row>
     <x:row r="143" spans="1:5">
       <x:c r="A143" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B143" s="0" t="n">
-        <x:v>413</x:v>
+        <x:v>405</x:v>
       </x:c>
       <x:c r="C143" s="0" t="s">
         <x:v>157</x:v>
       </x:c>
       <x:c r="D143" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E143" s="0" t="n">
-        <x:v>4500</x:v>
+        <x:v>1700</x:v>
       </x:c>
     </x:row>
     <x:row r="144" spans="1:5">
       <x:c r="A144" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B144" s="0" t="n">
-        <x:v>414</x:v>
+        <x:v>411</x:v>
       </x:c>
       <x:c r="C144" s="0" t="s">
         <x:v>158</x:v>
       </x:c>
       <x:c r="D144" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E144" s="0" t="n">
-        <x:v>1100</x:v>
+        <x:v>19000</x:v>
       </x:c>
     </x:row>
     <x:row r="145" spans="1:5">
       <x:c r="A145" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B145" s="0" t="n">
-        <x:v>415</x:v>
+        <x:v>412</x:v>
       </x:c>
       <x:c r="C145" s="0" t="s">
         <x:v>159</x:v>
       </x:c>
       <x:c r="D145" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E145" s="0" t="n">
-        <x:v>12500</x:v>
+        <x:v>25500</x:v>
       </x:c>
     </x:row>
     <x:row r="146" spans="1:5">
       <x:c r="A146" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="B146" s="0" t="n">
+        <x:v>413</x:v>
+      </x:c>
+      <x:c r="C146" s="0" t="s">
         <x:v>160</x:v>
       </x:c>
-      <x:c r="B146" s="0" t="n">
-        <x:v>241</x:v>
-      </x:c>
-      <x:c r="C146" s="0" t="s">
-        <x:v>161</x:v>
-      </x:c>
       <x:c r="D146" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E146" s="0" t="n">
-        <x:v>110000</x:v>
+        <x:v>4500</x:v>
       </x:c>
     </x:row>
     <x:row r="147" spans="1:5">
       <x:c r="A147" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B147" s="0" t="n">
-        <x:v>242</x:v>
+        <x:v>414</x:v>
       </x:c>
       <x:c r="C147" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="D147" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E147" s="0" t="n">
-        <x:v>92800</x:v>
+        <x:v>1100</x:v>
       </x:c>
     </x:row>
     <x:row r="148" spans="1:5">
       <x:c r="A148" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B148" s="0" t="n">
-        <x:v>243</x:v>
+        <x:v>415</x:v>
       </x:c>
       <x:c r="C148" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="D148" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E148" s="0" t="n">
-        <x:v>28400</x:v>
+        <x:v>15000</x:v>
       </x:c>
     </x:row>
     <x:row r="149" spans="1:5">
       <x:c r="A149" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="B149" s="0" t="n">
-        <x:v>244</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="C149" s="0" t="s">
         <x:v>164</x:v>
       </x:c>
       <x:c r="D149" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E149" s="0" t="n">
-        <x:v>66000</x:v>
+        <x:v>110000</x:v>
       </x:c>
     </x:row>
     <x:row r="150" spans="1:5">
       <x:c r="A150" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="B150" s="0" t="n">
-        <x:v>245</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="C150" s="0" t="s">
         <x:v>165</x:v>
       </x:c>
       <x:c r="D150" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E150" s="0" t="n">
-        <x:v>60800</x:v>
+        <x:v>104400</x:v>
       </x:c>
     </x:row>
     <x:row r="151" spans="1:5">
       <x:c r="A151" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="B151" s="0" t="n">
-        <x:v>246</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="C151" s="0" t="s">
         <x:v>166</x:v>
       </x:c>
       <x:c r="D151" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E151" s="0" t="n">
-        <x:v>73200</x:v>
+        <x:v>28400</x:v>
       </x:c>
     </x:row>
     <x:row r="152" spans="1:5">
       <x:c r="A152" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="B152" s="0" t="n">
+        <x:v>244</x:v>
+      </x:c>
+      <x:c r="C152" s="0" t="s">
         <x:v>167</x:v>
       </x:c>
-      <x:c r="B152" s="0" t="n">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="C152" s="0" t="s">
-        <x:v>168</x:v>
-      </x:c>
       <x:c r="D152" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E152" s="0" t="n">
-        <x:v>103500</x:v>
+        <x:v>66000</x:v>
       </x:c>
     </x:row>
     <x:row r="153" spans="1:5">
       <x:c r="A153" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="B153" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="C153" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D153" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E153" s="0" t="n">
-        <x:v>203000</x:v>
+        <x:v>60800</x:v>
       </x:c>
     </x:row>
     <x:row r="154" spans="1:5">
       <x:c r="A154" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="B154" s="0" t="n">
-        <x:v>219</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="C154" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="D154" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E154" s="0" t="n">
-        <x:v>179400</x:v>
+        <x:v>73200</x:v>
       </x:c>
     </x:row>
     <x:row r="155" spans="1:5">
@@ -3583,16 +3592,16 @@
         <x:v>170</x:v>
       </x:c>
       <x:c r="B155" s="0" t="n">
-        <x:v>220</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C155" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="D155" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E155" s="0" t="n">
-        <x:v>33600</x:v>
+        <x:v>103500</x:v>
       </x:c>
     </x:row>
     <x:row r="156" spans="1:5">
@@ -3600,279 +3609,279 @@
         <x:v>170</x:v>
       </x:c>
       <x:c r="B156" s="0" t="n">
-        <x:v>221</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C156" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="D156" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E156" s="0" t="n">
-        <x:v>28800</x:v>
+        <x:v>203000</x:v>
       </x:c>
     </x:row>
     <x:row r="157" spans="1:5">
       <x:c r="A157" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B157" s="0" t="n">
-        <x:v>222</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="C157" s="0" t="s">
         <x:v>174</x:v>
       </x:c>
       <x:c r="D157" s="0" t="n">
-        <x:v>39</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E157" s="0" t="n">
-        <x:v>226200</x:v>
+        <x:v>191100</x:v>
       </x:c>
     </x:row>
     <x:row r="158" spans="1:5">
       <x:c r="A158" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B158" s="0" t="n">
-        <x:v>223</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="C158" s="0" t="s">
         <x:v>175</x:v>
       </x:c>
       <x:c r="D158" s="0" t="n">
-        <x:v>74</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E158" s="0" t="n">
-        <x:v>666600</x:v>
+        <x:v>33600</x:v>
       </x:c>
     </x:row>
     <x:row r="159" spans="1:5">
       <x:c r="A159" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B159" s="0" t="n">
-        <x:v>224</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="C159" s="0" t="s">
         <x:v>176</x:v>
       </x:c>
       <x:c r="D159" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E159" s="0" t="n">
-        <x:v>558600</x:v>
+        <x:v>33600</x:v>
       </x:c>
     </x:row>
     <x:row r="160" spans="1:5">
       <x:c r="A160" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B160" s="0" t="n">
-        <x:v>225</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="C160" s="0" t="s">
         <x:v>177</x:v>
       </x:c>
       <x:c r="D160" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E160" s="0" t="n">
-        <x:v>259880</x:v>
+        <x:v>226200</x:v>
       </x:c>
     </x:row>
     <x:row r="161" spans="1:5">
       <x:c r="A161" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B161" s="0" t="n">
-        <x:v>226</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="C161" s="0" t="s">
         <x:v>178</x:v>
       </x:c>
       <x:c r="D161" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="E161" s="0" t="n">
-        <x:v>102400</x:v>
+        <x:v>694500</x:v>
       </x:c>
     </x:row>
     <x:row r="162" spans="1:5">
       <x:c r="A162" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="B162" s="0" t="n">
+        <x:v>224</x:v>
+      </x:c>
+      <x:c r="C162" s="0" t="s">
         <x:v>179</x:v>
       </x:c>
-      <x:c r="B162" s="0" t="n">
-        <x:v>290</x:v>
-      </x:c>
-      <x:c r="C162" s="0" t="s">
-        <x:v>180</x:v>
-      </x:c>
       <x:c r="D162" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="E162" s="0" t="n">
-        <x:v>15000</x:v>
+        <x:v>567900</x:v>
       </x:c>
     </x:row>
     <x:row r="163" spans="1:5">
       <x:c r="A163" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B163" s="0" t="n">
-        <x:v>291</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="C163" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="D163" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E163" s="0" t="n">
-        <x:v>90100</x:v>
+        <x:v>259880</x:v>
       </x:c>
     </x:row>
     <x:row r="164" spans="1:5">
       <x:c r="A164" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B164" s="0" t="n">
-        <x:v>292</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="C164" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="D164" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E164" s="0" t="n">
-        <x:v>32000</x:v>
+        <x:v>115300</x:v>
       </x:c>
     </x:row>
     <x:row r="165" spans="1:5">
       <x:c r="A165" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="B165" s="0" t="n">
-        <x:v>293</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="C165" s="0" t="s">
         <x:v>183</x:v>
       </x:c>
       <x:c r="D165" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E165" s="0" t="n">
-        <x:v>41100</x:v>
+        <x:v>22500</x:v>
       </x:c>
     </x:row>
     <x:row r="166" spans="1:5">
       <x:c r="A166" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="B166" s="0" t="n">
-        <x:v>294</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="C166" s="0" t="s">
         <x:v>184</x:v>
       </x:c>
       <x:c r="D166" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E166" s="0" t="n">
-        <x:v>32400</x:v>
+        <x:v>98400</x:v>
       </x:c>
     </x:row>
     <x:row r="167" spans="1:5">
       <x:c r="A167" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="B167" s="0" t="n">
-        <x:v>295</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="C167" s="0" t="s">
         <x:v>185</x:v>
       </x:c>
       <x:c r="D167" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E167" s="0" t="n">
-        <x:v>8500</x:v>
+        <x:v>48600</x:v>
       </x:c>
     </x:row>
     <x:row r="168" spans="1:5">
       <x:c r="A168" s="0" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="B168" s="0" t="n">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="C168" s="0" t="s">
         <x:v>186</x:v>
       </x:c>
-      <x:c r="B168" s="0" t="n">
-        <x:v>110</x:v>
-      </x:c>
-      <x:c r="C168" s="0" t="s">
-        <x:v>187</x:v>
-      </x:c>
       <x:c r="D168" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E168" s="0" t="n">
-        <x:v>158400</x:v>
+        <x:v>57700</x:v>
       </x:c>
     </x:row>
     <x:row r="169" spans="1:5">
       <x:c r="A169" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="B169" s="0" t="n">
-        <x:v>111</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="C169" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="D169" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E169" s="0" t="n">
-        <x:v>19800</x:v>
+        <x:v>40700</x:v>
       </x:c>
     </x:row>
     <x:row r="170" spans="1:5">
       <x:c r="A170" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="B170" s="0" t="n">
-        <x:v>112</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="C170" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="D170" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E170" s="0" t="n">
-        <x:v>102200</x:v>
+        <x:v>8500</x:v>
       </x:c>
     </x:row>
     <x:row r="171" spans="1:5">
       <x:c r="A171" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B171" s="0" t="n">
-        <x:v>113</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C171" s="0" t="s">
         <x:v>190</x:v>
       </x:c>
       <x:c r="D171" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E171" s="0" t="n">
-        <x:v>22800</x:v>
+        <x:v>158400</x:v>
       </x:c>
     </x:row>
     <x:row r="172" spans="1:5">
       <x:c r="A172" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B172" s="0" t="n">
-        <x:v>114</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C172" s="0" t="s">
         <x:v>191</x:v>
@@ -3881,176 +3890,227 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="E172" s="0" t="n">
-        <x:v>24600</x:v>
+        <x:v>19800</x:v>
       </x:c>
     </x:row>
     <x:row r="173" spans="1:5">
       <x:c r="A173" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B173" s="0" t="n">
-        <x:v>115</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C173" s="0" t="s">
         <x:v>192</x:v>
       </x:c>
       <x:c r="D173" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E173" s="0" t="n">
-        <x:v>82000</x:v>
+        <x:v>131400</x:v>
       </x:c>
     </x:row>
     <x:row r="174" spans="1:5">
       <x:c r="A174" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B174" s="0" t="n">
-        <x:v>116</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="C174" s="0" t="s">
         <x:v>193</x:v>
       </x:c>
       <x:c r="D174" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E174" s="0" t="n">
-        <x:v>45600</x:v>
+        <x:v>22800</x:v>
       </x:c>
     </x:row>
     <x:row r="175" spans="1:5">
       <x:c r="A175" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B175" s="0" t="n">
-        <x:v>117</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C175" s="0" t="s">
         <x:v>194</x:v>
       </x:c>
       <x:c r="D175" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E175" s="0" t="n">
-        <x:v>262200</x:v>
+        <x:v>24600</x:v>
       </x:c>
     </x:row>
     <x:row r="176" spans="1:5">
       <x:c r="A176" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B176" s="0" t="n">
-        <x:v>118</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="C176" s="0" t="s">
         <x:v>195</x:v>
       </x:c>
       <x:c r="D176" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E176" s="0" t="n">
-        <x:v>53200</x:v>
+        <x:v>82000</x:v>
       </x:c>
     </x:row>
     <x:row r="177" spans="1:5">
       <x:c r="A177" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B177" s="0" t="n">
-        <x:v>119</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C177" s="0" t="s">
         <x:v>196</x:v>
       </x:c>
       <x:c r="D177" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E177" s="0" t="n">
-        <x:v>62400</x:v>
+        <x:v>45600</x:v>
       </x:c>
     </x:row>
     <x:row r="178" spans="1:5">
       <x:c r="A178" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B178" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="C178" s="0" t="s">
         <x:v>197</x:v>
       </x:c>
       <x:c r="D178" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E178" s="0" t="n">
-        <x:v>8500</x:v>
+        <x:v>282900</x:v>
       </x:c>
     </x:row>
     <x:row r="179" spans="1:5">
       <x:c r="A179" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B179" s="0" t="n">
-        <x:v>121</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="C179" s="0" t="s">
         <x:v>198</x:v>
       </x:c>
       <x:c r="D179" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E179" s="0" t="n">
-        <x:v>53400</x:v>
+        <x:v>68400</x:v>
       </x:c>
     </x:row>
     <x:row r="180" spans="1:5">
       <x:c r="A180" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B180" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="C180" s="0" t="s">
         <x:v>199</x:v>
       </x:c>
       <x:c r="D180" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E180" s="0" t="n">
-        <x:v>64800</x:v>
+        <x:v>70200</x:v>
       </x:c>
     </x:row>
     <x:row r="181" spans="1:5">
       <x:c r="A181" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B181" s="0" t="n">
-        <x:v>123</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C181" s="0" t="s">
         <x:v>200</x:v>
       </x:c>
       <x:c r="D181" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E181" s="0" t="n">
-        <x:v>48600</x:v>
+        <x:v>25500</x:v>
       </x:c>
     </x:row>
     <x:row r="182" spans="1:5">
       <x:c r="A182" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B182" s="0" t="n">
-        <x:v>999999</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="C182" s="0" t="s">
         <x:v>201</x:v>
       </x:c>
       <x:c r="D182" s="0" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E182" s="0" t="n">
+        <x:v>80100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="183" spans="1:5">
+      <x:c r="A183" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="B183" s="0" t="n">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="C183" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="D183" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E183" s="0" t="n">
+        <x:v>64800</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="184" spans="1:5">
+      <x:c r="A184" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="B184" s="0" t="n">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="C184" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="D184" s="0" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E184" s="0" t="n">
+        <x:v>48600</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="185" spans="1:5">
+      <x:c r="A185" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="B185" s="0" t="n">
+        <x:v>999999</x:v>
+      </x:c>
+      <x:c r="C185" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="D185" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="E182" s="0" t="n">
+      <x:c r="E185" s="0" t="n">
         <x:v>-72419</x:v>
       </x:c>
     </x:row>

</xml_diff>